<commit_message>
updated case to include DIO-timestamped and revised NGCHP
</commit_message>
<xml_diff>
--- a/DistributionSystems/SimulinkOpal/Canary/relay_settings/relay_parameters.xlsx
+++ b/DistributionSystems/SimulinkOpal/Canary/relay_settings/relay_parameters.xlsx
@@ -735,7 +735,7 @@
   <dimension ref="A1:V9"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G4" sqref="G4"/>
+      <selection activeCell="H4" sqref="H4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -849,7 +849,7 @@
         <v>0.5</v>
       </c>
       <c r="G2" s="7">
-        <v>600</v>
+        <v>1200</v>
       </c>
       <c r="H2" s="10">
         <v>1</v>
@@ -861,7 +861,7 @@
         <v>0</v>
       </c>
       <c r="K2" s="7">
-        <v>0.8</v>
+        <v>0.5</v>
       </c>
       <c r="L2" s="7">
         <v>1</v>
@@ -870,10 +870,10 @@
         <v>1</v>
       </c>
       <c r="N2" s="7">
-        <v>0.9</v>
+        <v>0.8</v>
       </c>
       <c r="O2" s="7">
-        <v>1.1000000000000001</v>
+        <v>1.2</v>
       </c>
       <c r="P2" s="7">
         <v>20</v>
@@ -917,7 +917,7 @@
         <v>0.5</v>
       </c>
       <c r="G3" s="7">
-        <v>600</v>
+        <v>1200</v>
       </c>
       <c r="H3" s="10">
         <v>1</v>
@@ -929,7 +929,7 @@
         <v>0</v>
       </c>
       <c r="K3" s="7">
-        <v>0.8</v>
+        <v>0.5</v>
       </c>
       <c r="L3" s="7">
         <v>1</v>
@@ -938,10 +938,10 @@
         <v>1</v>
       </c>
       <c r="N3" s="7">
-        <v>0.9</v>
+        <v>0.8</v>
       </c>
       <c r="O3" s="7">
-        <v>1.1000000000000001</v>
+        <v>1.2</v>
       </c>
       <c r="P3" s="7">
         <v>20</v>

</xml_diff>